<commit_message>
changes Made in userPage
</commit_message>
<xml_diff>
--- a/Skad_HRMS/src/main/java/hrms/qa/TestData/TestData.xlsx
+++ b/Skad_HRMS/src/main/java/hrms/qa/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="6350"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>FirstName</t>
   </si>
@@ -74,6 +74,39 @@
     <t>tempaddress</t>
   </si>
   <si>
+    <t>JobTitle</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Sub Dep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmploymentType
+</t>
+  </si>
+  <si>
+    <t>EmployedThrough</t>
+  </si>
+  <si>
+    <t>WorkMode</t>
+  </si>
+  <si>
+    <t>Work Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VendorName
+</t>
+  </si>
+  <si>
+    <t>BillingType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserTimezone
+</t>
+  </si>
+  <si>
     <t>Arun</t>
   </si>
   <si>
@@ -111,6 +144,33 @@
   </si>
   <si>
     <t>skdafjhbdsjdskahfliua</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Contractor - hourly</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Skad</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>Australia/South</t>
   </si>
 </sst>
 </file>
@@ -123,7 +183,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +198,12 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF0A0D14"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -605,134 +671,134 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -741,6 +807,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1275,10 +1347,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1298,9 +1370,19 @@
     <col min="13" max="13" width="10.6363636363636" customWidth="1"/>
     <col min="14" max="14" width="18.9090909090909" customWidth="1"/>
     <col min="15" max="15" width="19.7272727272727" customWidth="1"/>
+    <col min="16" max="16" width="13.2727272727273" customWidth="1"/>
+    <col min="17" max="17" width="13.9090909090909" customWidth="1"/>
+    <col min="18" max="18" width="12.2727272727273" customWidth="1"/>
+    <col min="19" max="19" width="17.6363636363636" customWidth="1"/>
+    <col min="20" max="20" width="17.7272727272727" customWidth="1"/>
+    <col min="21" max="21" width="18.0909090909091" customWidth="1"/>
+    <col min="22" max="22" width="14.4545454545455" customWidth="1"/>
+    <col min="23" max="23" width="15.1818181818182" customWidth="1"/>
+    <col min="24" max="24" width="19.2727272727273" customWidth="1"/>
+    <col min="25" max="25" width="14.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" ht="45" customHeight="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1346,52 +1428,109 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G2">
         <v>4362436436</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M2">
         <v>614625</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="P2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes made in departments,baseclass,user
</commit_message>
<xml_diff>
--- a/Skad_HRMS/src/main/java/hrms/qa/TestData/TestData.xlsx
+++ b/Skad_HRMS/src/main/java/hrms/qa/TestData/TestData.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6350"/>
+    <workbookView windowWidth="18350" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="ProjectData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>FirstName</t>
   </si>
@@ -171,6 +172,79 @@
   </si>
   <si>
     <t>Australia/South</t>
+  </si>
+  <si>
+    <t>Project No</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Project Type</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Sub Department</t>
+  </si>
+  <si>
+    <t>Members</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Name
+</t>
+  </si>
+  <si>
+    <t>Project Description</t>
+  </si>
+  <si>
+    <t>Jira Project URL</t>
+  </si>
+  <si>
+    <t>Project Starting Date</t>
+  </si>
+  <si>
+    <t>Project End Date</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Notify At</t>
+  </si>
+  <si>
+    <t>Estimated Hrs</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Billable</t>
+  </si>
+  <si>
+    <t>Allen Paul</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Creation </t>
+  </si>
+  <si>
+    <t>[SS-124] The data was missing on the website. - Jira</t>
+  </si>
+  <si>
+    <t>20/12/2024</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>30/12/2024</t>
   </si>
 </sst>
 </file>
@@ -183,20 +257,12 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,6 +270,41 @@
       <color rgb="FF0A0D14"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -668,151 +769,166 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1089,6 +1205,101 @@
 </styleSheet>
 </file>
 
+<file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{00000000-0000-0000-0000-000000000000}" r:id="rId1" ax:persistence="persistStreamInit"/>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{00000000-0000-0000-0000-000000000000}" r:id="rId1" ax:persistence="persistStreamInit"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1397000</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Host Control  5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8318500" y="0"/>
+              <a:ext cx="1397000" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1397000</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp>
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Host Control  6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8318500" y="368300"/>
+              <a:ext cx="1397000" cy="184150"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1349,8 +1560,8 @@
   <sheetPr/>
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1428,16 +1639,16 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">
@@ -1446,16 +1657,16 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1469,10 +1680,10 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
@@ -1481,10 +1692,10 @@
       <c r="G2">
         <v>4362436436</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="J2" t="s">
@@ -1510,6 +1721,9 @@
       </c>
       <c r="Q2" t="s">
         <v>39</v>
+      </c>
+      <c r="R2" t="s">
+        <v>38</v>
       </c>
       <c r="S2" t="s">
         <v>40</v>
@@ -1541,4 +1755,209 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="15.9090909090909" customWidth="1"/>
+    <col min="2" max="2" width="17.0909090909091" customWidth="1"/>
+    <col min="3" max="3" width="19.2727272727273" customWidth="1"/>
+    <col min="4" max="4" width="24.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="22.3636363636364" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="25.2727272727273" customWidth="1"/>
+    <col min="8" max="8" width="15.5454545454545" customWidth="1"/>
+    <col min="9" max="9" width="14.8181818181818" customWidth="1"/>
+    <col min="10" max="10" width="19.4545454545455" customWidth="1"/>
+    <col min="11" max="11" width="43.6363636363636" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="15" width="12.4545454545455" customWidth="1"/>
+    <col min="16" max="16" width="17.6363636363636" customWidth="1"/>
+    <col min="17" max="17" width="16.7272727272727" customWidth="1"/>
+    <col min="18" max="18" width="19.5454545454545" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="29" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="6">
+        <v>45609</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" ht="15.5" spans="7:7">
+      <c r="G3" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId5" display="[SS-124] The data was missing on the website. - Jira" tooltip="https://hexagon84020.atlassian.net/browse/SS-124?focusedCommentId=28939"/>
+    <hyperlink ref="L2" r:id="rId5" display="45609" tooltip="https://hexagon84020.atlassian.net/browse/SS-124?focusedCommentId=28939"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <controls>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId3">
+          <controlPr defaultSize="0">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1397000</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId4">
+          <controlPr defaultSize="0">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>1397000</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </controls>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes made in user ,base ,departments
</commit_message>
<xml_diff>
--- a/Skad_HRMS/src/main/java/hrms/qa/TestData/TestData.xlsx
+++ b/Skad_HRMS/src/main/java/hrms/qa/TestData/TestData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="ProjectData" sheetId="2" r:id="rId2"/>
+    <sheet name="VendorAdministration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t>FirstName</t>
   </si>
@@ -245,6 +246,39 @@
   </si>
   <si>
     <t>30/12/2024</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>PermanentAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolphin </t>
+  </si>
+  <si>
+    <t>dolphin@gmail.com</t>
+  </si>
+  <si>
+    <t>3 North street Orathanadu</t>
   </si>
 </sst>
 </file>
@@ -266,6 +300,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color rgb="FF0A0D14"/>
       <name val="Arial"/>
@@ -297,14 +339,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -769,7 +803,7 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -903,7 +937,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -912,7 +946,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -921,13 +958,10 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1560,7 +1594,7 @@
   <sheetPr/>
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -1639,16 +1673,16 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="T1" t="s">
@@ -1657,16 +1691,16 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1680,10 +1714,10 @@
       <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F2" t="s">
@@ -1692,10 +1726,10 @@
       <c r="G2">
         <v>4362436436</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J2" t="s">
@@ -1789,58 +1823,58 @@
   </cols>
   <sheetData>
     <row r="1" ht="29" spans="1:18">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Q1" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="7"/>
+      <c r="R1" s="8"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2">
@@ -1861,7 +1895,7 @@
       <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>64</v>
       </c>
       <c r="H2" t="s">
@@ -1876,7 +1910,7 @@
       <c r="K2" t="s">
         <v>67</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="7">
         <v>45609</v>
       </c>
       <c r="M2" t="s">
@@ -1896,7 +1930,7 @@
       </c>
     </row>
     <row r="3" ht="15.5" spans="7:7">
-      <c r="G3" s="4"/>
+      <c r="G3" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1960,4 +1994,86 @@
     </mc:AlternateContent>
   </controls>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="19.2727272727273" customWidth="1"/>
+    <col min="2" max="2" width="21.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="16.9090909090909" customWidth="1"/>
+    <col min="4" max="4" width="13.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="18.5454545454545" customWidth="1"/>
+    <col min="6" max="6" width="14.8181818181818" customWidth="1"/>
+    <col min="7" max="7" width="17.6363636363636" customWidth="1"/>
+    <col min="8" max="8" width="25.3636363636364" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2">
+        <v>9159268812</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>614625</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="dolphin@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>